<commit_message>
update backlog and user stories
</commit_message>
<xml_diff>
--- a/doc/Scrum Backlog.xlsx
+++ b/doc/Scrum Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/kandathi_ualberta_ca/Documents/2019 Fall/CMPUT 301/FindMyFeelings/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamne\OneDrive - ualberta.ca\2019 Fall\CMPUT 301\FindMyFeelings\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CDAAB5C-F5EF-4179-BEFF-6E6EF345A04B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{8CDAAB5C-F5EF-4179-BEFF-6E6EF345A04B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9DCCA5FF-882F-4679-9326-40176FD90AD1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{451405E6-5B18-4C5C-A949-49A613745B1C}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7810" xr2:uid="{451405E6-5B18-4C5C-A949-49A613745B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>TASK</t>
   </si>
@@ -45,12 +45,6 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>Class Profile</t>
-  </si>
-  <si>
-    <t>Class Mood</t>
-  </si>
-  <si>
     <t>View Mood Event</t>
   </si>
   <si>
@@ -100,22 +94,59 @@
   </si>
   <si>
     <t>Add optional location in ADD MOOD</t>
+  </si>
+  <si>
+    <t>Nevil</t>
+  </si>
+  <si>
+    <t>Ramy</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Travis</t>
+  </si>
+  <si>
+    <t>Not complete</t>
+  </si>
+  <si>
+    <t>Profile Activity</t>
+  </si>
+  <si>
+    <t>Josh/Ramy</t>
+  </si>
+  <si>
+    <t>Nevil/Sandy/Cameron</t>
+  </si>
+  <si>
+    <t>Ramy/Josh</t>
+  </si>
+  <si>
+    <t>Travis/Nevil</t>
+  </si>
+  <si>
+    <t>Sandy/Nevil/Cameron</t>
+  </si>
+  <si>
+    <t>Map Activity</t>
+  </si>
+  <si>
+    <t>User Class, Mood Class</t>
+  </si>
+  <si>
+    <t>HomePage Activity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,11 +163,32 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="18"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Utsaah"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -171,21 +223,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -194,6 +255,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA50021"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -502,37 +568,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F15BC3F-1D30-4068-AC32-E059106A13FD}">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="76" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.90625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.5">
@@ -542,136 +608,293 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.6">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.6">
+      <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.6">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.6">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.6">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="36.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7">
+        <v>43755</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="8">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="40" x14ac:dyDescent="0.6">
+      <c r="A17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="8">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.6">
+      <c r="A18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="8">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="8">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="40" x14ac:dyDescent="0.6">
+      <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="B23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="8">
+        <v>43784</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.6">
+      <c r="A24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="8">
+        <v>43784</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="40" x14ac:dyDescent="0.6">
+      <c r="A25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="8">
+        <v>43784</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005DA220EE64769F47A6DFBFD9BF15B0CA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e049abba3f8f63cba6e367b367898a73">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b0d59e1e-f34f-4563-8590-b012a460d4b6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3d4e1189dcacfb4d83aa385aec72d5" ns3:_="">
     <xsd:import namespace="b0d59e1e-f34f-4563-8590-b012a460d4b6"/>
@@ -835,22 +1058,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D9D1FE-CDD5-404A-8793-56ABB79A6871}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b0d59e1e-f34f-4563-8590-b012a460d4b6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA813A07-D1BE-4D67-9285-C32EFF6FFA2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D2633D7-F434-4AC3-9149-20883911640D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -866,28 +1098,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA813A07-D1BE-4D67-9285-C32EFF6FFA2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D9D1FE-CDD5-404A-8793-56ABB79A6871}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b0d59e1e-f34f-4563-8590-b012a460d4b6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>